<commit_message>
apos testes feitos no pc escritorio
</commit_message>
<xml_diff>
--- a/BaseMotoristas.xlsx
+++ b/BaseMotoristas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,6 +1110,96 @@
         <v>620696</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>AUK0451</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ARIOVALDO SOUZA GOMES</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>620578</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DDY4C74</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MARIO ROBERTO</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>620686</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>DPE0B20</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>DAVID DE JESUS</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>619353</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>EAR7C31</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>LEONARDO MAGALHAES</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>620867</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GHG7C42</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>RODOLFO PIZANI</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>436321</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>IWJ4B20</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>DAVID DE JESUS</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>619353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feito ajustes pra rodar no csc
</commit_message>
<xml_diff>
--- a/BaseMotoristas.xlsx
+++ b/BaseMotoristas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="119">
   <si>
     <t>PLACA</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>AQH*5643</t>
+  </si>
+  <si>
+    <t>FKK4G59</t>
   </si>
   <si>
     <t>CARLOS ROBERTO DA SILVA</t>
@@ -725,7 +728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -747,7 +750,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>619651</v>
@@ -758,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>66</v>
@@ -769,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4">
         <v>66</v>
@@ -780,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>620578</v>
@@ -791,7 +794,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6">
         <v>620265</v>
@@ -802,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>620578</v>
@@ -813,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8">
         <v>436394</v>
@@ -824,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>120</v>
@@ -835,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10">
         <v>619520</v>
@@ -846,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C11">
         <v>619840</v>
@@ -857,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12">
         <v>620724</v>
@@ -868,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13">
         <v>620820</v>
@@ -879,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>620820</v>
@@ -890,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>436267</v>
@@ -901,7 +904,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16">
         <v>620487</v>
@@ -912,7 +915,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C17">
         <v>620447</v>
@@ -923,7 +926,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>620529</v>
@@ -934,7 +937,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>620686</v>
@@ -945,7 +948,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C20">
         <v>619609</v>
@@ -956,7 +959,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21">
         <v>1213</v>
@@ -967,7 +970,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22">
         <v>2044</v>
@@ -978,7 +981,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23">
         <v>619353</v>
@@ -989,7 +992,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24">
         <v>620487</v>
@@ -1000,7 +1003,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <v>620385</v>
@@ -1011,7 +1014,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26">
         <v>620696</v>
@@ -1022,7 +1025,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C27">
         <v>620867</v>
@@ -1033,7 +1036,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C28">
         <v>620326</v>
@@ -1044,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29">
         <v>263</v>
@@ -1055,7 +1058,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30">
         <v>620904</v>
@@ -1066,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>1140</v>
@@ -1077,7 +1080,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32">
         <v>619886</v>
@@ -1088,7 +1091,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33">
         <v>619859</v>
@@ -1099,7 +1102,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C34">
         <v>1140</v>
@@ -1110,7 +1113,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35">
         <v>620319</v>
@@ -1121,7 +1124,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36">
         <v>620319</v>
@@ -1132,7 +1135,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C37">
         <v>436634</v>
@@ -1143,7 +1146,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C38">
         <v>620153</v>
@@ -1154,7 +1157,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C39">
         <v>620225</v>
@@ -1165,7 +1168,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C40">
         <v>620960</v>
@@ -1176,7 +1179,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C41">
         <v>619743</v>
@@ -1187,7 +1190,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>436264</v>
@@ -1198,7 +1201,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C43">
         <v>436418</v>
@@ -1209,7 +1212,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>121</v>
@@ -1220,7 +1223,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C45">
         <v>619812</v>
@@ -1231,7 +1234,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46">
         <v>436321</v>
@@ -1242,7 +1245,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C47">
         <v>619883</v>
@@ -1253,7 +1256,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C48">
         <v>1650</v>
@@ -1264,7 +1267,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49">
         <v>619801</v>
@@ -1275,7 +1278,7 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C50">
         <v>620754</v>
@@ -1286,7 +1289,7 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C51">
         <v>619801</v>
@@ -1297,7 +1300,7 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C52">
         <v>619353</v>
@@ -1308,7 +1311,7 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C53">
         <v>436618</v>
@@ -1319,7 +1322,7 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C54">
         <v>619951</v>
@@ -1330,7 +1333,7 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C55">
         <v>104</v>
@@ -1341,7 +1344,7 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56">
         <v>619724</v>
@@ -1352,7 +1355,7 @@
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C57">
         <v>620754</v>
@@ -1363,7 +1366,7 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C58">
         <v>619388</v>
@@ -1374,7 +1377,7 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C59">
         <v>620894</v>
@@ -1385,7 +1388,7 @@
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C60">
         <v>118</v>
@@ -1396,7 +1399,7 @@
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C61">
         <v>619860</v>
@@ -1407,7 +1410,7 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C62">
         <v>620970</v>
@@ -1418,7 +1421,7 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C63">
         <v>620937</v>
@@ -1429,7 +1432,7 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C64">
         <v>620972</v>
@@ -1440,10 +1443,65 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C65">
         <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66">
+        <v>619883</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67">
+        <v>619883</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68">
+        <v>619883</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69">
+        <v>619883</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70">
+        <v>619609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>